<commit_message>
Nymph to adult update.
</commit_message>
<xml_diff>
--- a/data/egg_tube_data.xlsx
+++ b/data/egg_tube_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasiabernat/Desktop/git_repositories/extreme-flight-trials/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7FDC85-7293-AD45-970C-B5948DE49C22}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF41E78-75DB-1D41-BA73-6432DFA5AD8E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="180" yWindow="500" windowWidth="27280" windowHeight="16620" xr2:uid="{CE040209-3C16-F54B-BD28-83BB5606938B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4446" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4458" uniqueCount="75">
   <si>
     <t>gen1_ID</t>
   </si>
@@ -247,6 +247,9 @@
   </si>
   <si>
     <t>10.16-10.18</t>
+  </si>
+  <si>
+    <t>10.19.21</t>
   </si>
 </sst>
 </file>
@@ -700,8 +703,8 @@
   <dimension ref="A1:L1276"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A740" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G768" sqref="G768"/>
+      <pane ySplit="1" topLeftCell="A684" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H692" sqref="H692"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -20483,13 +20486,19 @@
         <v>38</v>
       </c>
       <c r="D691" s="8"/>
-      <c r="E691" s="8"/>
+      <c r="E691" s="8" t="s">
+        <v>74</v>
+      </c>
       <c r="F691" s="8"/>
       <c r="G691" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H691" s="8"/>
-      <c r="I691" s="8"/>
+      <c r="H691" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I691" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="J691" s="8"/>
       <c r="K691" s="8"/>
     </row>
@@ -21121,13 +21130,19 @@
       <c r="D713" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E713" s="6"/>
+      <c r="E713" s="6" t="s">
+        <v>74</v>
+      </c>
       <c r="F713" s="6"/>
       <c r="G713" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H713" s="6"/>
-      <c r="I713" s="6"/>
+      <c r="H713" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I713" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="J713" s="11" t="s">
         <v>30</v>
       </c>
@@ -22348,13 +22363,19 @@
       <c r="D759" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E759" s="6"/>
+      <c r="E759" s="6" t="s">
+        <v>74</v>
+      </c>
       <c r="F759" s="6"/>
       <c r="G759" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H759" s="6"/>
-      <c r="I759" s="6"/>
+      <c r="H759" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I759" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="J759" s="6"/>
       <c r="K759" s="6"/>
     </row>
@@ -22454,13 +22475,19 @@
       <c r="D763" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E763" s="6"/>
+      <c r="E763" s="6" t="s">
+        <v>74</v>
+      </c>
       <c r="F763" s="6"/>
       <c r="G763" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H763" s="6"/>
-      <c r="I763" s="6"/>
+      <c r="H763" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I763" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="J763" s="6"/>
       <c r="K763" s="6"/>
     </row>

</xml_diff>

<commit_message>
Update on nymphs to adults except for one.
</commit_message>
<xml_diff>
--- a/data/egg_tube_data.xlsx
+++ b/data/egg_tube_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasiabernat/Desktop/git_repositories/extreme-flight-trials/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF41E78-75DB-1D41-BA73-6432DFA5AD8E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA7AC66-A315-D141-ACC0-20D2D181A301}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="180" yWindow="500" windowWidth="27280" windowHeight="16620" xr2:uid="{CE040209-3C16-F54B-BD28-83BB5606938B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4458" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4469" uniqueCount="80">
   <si>
     <t>gen1_ID</t>
   </si>
@@ -250,6 +250,21 @@
   </si>
   <si>
     <t>10.19.21</t>
+  </si>
+  <si>
+    <t>10.20.21</t>
+  </si>
+  <si>
+    <t>10.25.21</t>
+  </si>
+  <si>
+    <t>10.23-10.25</t>
+  </si>
+  <si>
+    <t>10.22.21</t>
+  </si>
+  <si>
+    <t>pending</t>
   </si>
 </sst>
 </file>
@@ -703,8 +718,8 @@
   <dimension ref="A1:L1276"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A684" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H692" sqref="H692"/>
+      <pane ySplit="1" topLeftCell="A737" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K750" sqref="K750"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -21312,13 +21327,19 @@
       <c r="D720" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E720" s="6"/>
+      <c r="E720" s="6" t="s">
+        <v>78</v>
+      </c>
       <c r="F720" s="6"/>
       <c r="G720" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H720" s="6"/>
-      <c r="I720" s="6"/>
+      <c r="H720" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I720" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="J720" s="11" t="s">
         <v>30</v>
       </c>
@@ -22108,13 +22129,19 @@
       <c r="D750" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E750" s="6"/>
+      <c r="E750" s="6" t="s">
+        <v>75</v>
+      </c>
       <c r="F750" s="6"/>
       <c r="G750" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H750" s="6"/>
-      <c r="I750" s="6"/>
+      <c r="H750" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I750" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="J750" s="6"/>
       <c r="K750" s="6"/>
     </row>
@@ -22131,15 +22158,23 @@
       <c r="D751" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E751" s="6"/>
+      <c r="E751" s="6" t="s">
+        <v>76</v>
+      </c>
       <c r="F751" s="6"/>
       <c r="G751" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H751" s="6"/>
-      <c r="I751" s="6"/>
+      <c r="H751" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I751" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="J751" s="6"/>
-      <c r="K751" s="6"/>
+      <c r="K751" s="6" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="752" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A752" s="6">
@@ -22392,7 +22427,9 @@
       <c r="D760" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E760" s="6"/>
+      <c r="E760" s="6" t="s">
+        <v>79</v>
+      </c>
       <c r="F760" s="6"/>
       <c r="G760" s="11" t="s">
         <v>18</v>

</xml_diff>